<commit_message>
Update Product Back Log and Sprint Back Log
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 3/SixGuys_Deliverable_3_ProductBackLog_4.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 3/SixGuys_Deliverable_3_ProductBackLog_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Umaine\COS420\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EC7E65-4FF4-4D24-872A-F32D5498E28C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D9698D-C8FB-4E1D-B698-C2BCDE7C80C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1598,7 @@
         <v>80</v>
       </c>
       <c r="E29" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Update sprint back log for cooper
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 3/SixGuys_Deliverable_3_ProductBackLog_4.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 3/SixGuys_Deliverable_3_ProductBackLog_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Umaine\COS420\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D9698D-C8FB-4E1D-B698-C2BCDE7C80C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316E2664-AA8B-4060-83A0-8B4EA5478C7D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
   <si>
     <t>Sprint Number</t>
   </si>
@@ -274,6 +274,26 @@
   </si>
   <si>
     <t>As a player, I want to be able to fight against a variety of enemies so that I do not get bored with having to kill the same enemies repeatedly for the whole game.</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>As a player I want to be able to lose lives so that the game has risks in it.</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>As a player I want to be able to get a gameover so that I can lose the game.</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Gameplay_14</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Gameplay_15</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -496,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -536,9 +556,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -580,15 +597,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Input" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
     <dxf>
       <font>
-        <b/>
+        <color theme="8"/>
       </font>
     </dxf>
     <dxf>
@@ -610,6 +633,31 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,16 +741,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:F35" totalsRowShown="0">
-  <autoFilter ref="A1:F35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
-    <sortCondition ref="C2:C35" customList="H,M,L"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:F37" totalsRowShown="0">
+  <autoFilter ref="A1:F37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
+    <sortCondition ref="C1:C37" customList="H,M,L"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Sprint Number"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ID"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Story Priority"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Story Status" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Story Status" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Story Points"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="User Story"/>
   </tableColumns>
@@ -1007,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F23" sqref="F23:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1066,7 @@
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="19" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="23" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="174.85546875" style="1" customWidth="1"/>
     <col min="7" max="1024" width="9.140625" style="1"/>
@@ -1034,7 +1082,7 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -1045,7 +1093,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1054,7 +1102,7 @@
       <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="9">
@@ -1066,7 +1114,7 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1075,7 +1123,7 @@
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="9">
@@ -1087,7 +1135,7 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="32">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1096,7 +1144,7 @@
       <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="9">
@@ -1108,7 +1156,7 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
+      <c r="A5" s="32">
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -1117,7 +1165,7 @@
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>79</v>
       </c>
       <c r="E5" s="9">
@@ -1129,7 +1177,7 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+      <c r="A6" s="32">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1138,7 +1186,7 @@
       <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="9">
@@ -1150,7 +1198,7 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
+      <c r="A7" s="32">
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -1159,7 +1207,7 @@
       <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="9">
@@ -1171,7 +1219,7 @@
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
+      <c r="A8" s="32">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1180,7 +1228,7 @@
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="9">
@@ -1192,7 +1240,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
+      <c r="A9" s="32">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1201,7 +1249,7 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="9">
@@ -1213,7 +1261,7 @@
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="33">
+      <c r="A10" s="32">
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1222,7 +1270,7 @@
       <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="9">
@@ -1234,7 +1282,7 @@
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
+      <c r="A11" s="33">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1243,7 +1291,7 @@
       <c r="C11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="29" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4">
@@ -1262,7 +1310,7 @@
       <c r="C12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="9">
@@ -1281,7 +1329,7 @@
       <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="9">
@@ -1302,7 +1350,7 @@
       <c r="C14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="9">
@@ -1323,7 +1371,7 @@
       <c r="C15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="9">
@@ -1342,7 +1390,7 @@
       <c r="C16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="9">
@@ -1361,7 +1409,7 @@
       <c r="C17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="9">
@@ -1380,7 +1428,7 @@
       <c r="C18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="9">
@@ -1399,7 +1447,7 @@
       <c r="C19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="9">
@@ -1418,7 +1466,7 @@
       <c r="C20" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="9">
@@ -1439,7 +1487,7 @@
       <c r="C21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="20" t="s">
         <v>80</v>
       </c>
       <c r="E21" s="9">
@@ -1460,7 +1508,7 @@
       <c r="C22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="20" t="s">
         <v>80</v>
       </c>
       <c r="E22" s="9">
@@ -1472,257 +1520,296 @@
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="4">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="4">
+        <v>5</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="9">
-        <v>5</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="9">
-        <v>1</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>4</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="25" t="s">
-        <v>11</v>
+      <c r="D25" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="E25" s="9">
         <v>5</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
-      <c r="B26" s="28" t="s">
-        <v>56</v>
+      <c r="B26" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="32">
-        <v>2</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>57</v>
+      <c r="E26" s="31">
+        <v>1</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15" t="s">
-        <v>58</v>
+      <c r="A27" s="14">
+        <v>4</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="17">
-        <v>2</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>59</v>
+      <c r="D27" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="31">
+        <v>5</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
-      <c r="B28" s="15" t="s">
-        <v>60</v>
+      <c r="B28" s="27" t="s">
+        <v>56</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="17">
-        <v>5</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>61</v>
+      <c r="E28" s="31">
+        <v>2</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <v>4</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>62</v>
+      <c r="A29" s="14"/>
+      <c r="B29" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>80</v>
+      <c r="D29" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="E29" s="17">
         <v>2</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="7" t="s">
-        <v>64</v>
+      <c r="B30" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E30" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="28" t="s">
-        <v>66</v>
+      <c r="A31" s="14">
+        <v>4</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>28</v>
+      <c r="D31" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="E31" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
-      <c r="B32" s="15" t="s">
-        <v>68</v>
+      <c r="B32" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
-      <c r="B33" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="19" t="s">
+      <c r="B33" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
-      <c r="B34" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="22" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="16" t="s">
+      <c r="A35" s="25"/>
+      <c r="B35" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="30" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="17">
         <v>3</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F35" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="17">
+        <v>2</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="17">
+        <v>3</v>
+      </c>
+      <c r="F37" s="26" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"IP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"W"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>